<commit_message>
Commiting new results of both
</commit_message>
<xml_diff>
--- a/EDGE.xlsx
+++ b/EDGE.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>problem</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>d1655</t>
+  </si>
+  <si>
+    <t>&gt;24hrs</t>
   </si>
 </sst>
 </file>
@@ -502,7 +505,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,6 +650,15 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
+      <c r="B9">
+        <v>8000</v>
+      </c>
+      <c r="C9">
+        <v>77</v>
+      </c>
+      <c r="D9">
+        <v>2530</v>
+      </c>
       <c r="E9">
         <v>2323</v>
       </c>
@@ -655,6 +667,15 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
+      <c r="B10">
+        <v>6746.3137140274002</v>
+      </c>
+      <c r="C10">
+        <v>71</v>
+      </c>
+      <c r="D10">
+        <v>16326</v>
+      </c>
       <c r="E10">
         <v>15780</v>
       </c>
@@ -671,6 +692,15 @@
       <c r="A12" t="s">
         <v>15</v>
       </c>
+      <c r="B12">
+        <v>42547.000015020298</v>
+      </c>
+      <c r="C12">
+        <v>106</v>
+      </c>
+      <c r="D12">
+        <v>12603</v>
+      </c>
       <c r="E12">
         <v>11861</v>
       </c>
@@ -678,6 +708,15 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>200</v>
+      </c>
+      <c r="D13">
+        <v>36101</v>
       </c>
       <c r="E13">
         <v>34643</v>

</xml_diff>